<commit_message>
Admin Settings UI, Backend modify acdemic year, department relations logic
</commit_message>
<xml_diff>
--- a/Sample Data/Teachers_list.xlsx
+++ b/Sample Data/Teachers_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oudai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Exam-Managment-Project\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA595D6-A4A3-4C6B-A750-883DDC36295C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB45735-C4E0-4B53-AFB9-009EC3F3DA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="19632" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>adj</t>
   </si>
@@ -121,150 +121,9 @@
     <t>Amina</t>
   </si>
   <si>
-    <t>Zerrouki</t>
-  </si>
-  <si>
-    <t>48291007</t>
-  </si>
-  <si>
-    <t>Networks &amp; Telecommunications</t>
-  </si>
-  <si>
-    <t>0654321993</t>
-  </si>
-  <si>
-    <t>amina.zerrouki@univ-alger.dz</t>
-  </si>
-  <si>
-    <t>Samir</t>
-  </si>
-  <si>
-    <t>Merbah</t>
-  </si>
-  <si>
-    <t>48291006</t>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
-    <t>Information Systems</t>
-  </si>
-  <si>
-    <t>0654321992</t>
-  </si>
-  <si>
-    <t>samir.merbah@univ-alger.dz</t>
-  </si>
-  <si>
-    <t>Nadia</t>
-  </si>
-  <si>
-    <t>Saadi</t>
-  </si>
-  <si>
-    <t>48291005</t>
-  </si>
-  <si>
-    <t>Game Development</t>
-  </si>
-  <si>
-    <t>0654321991</t>
-  </si>
-  <si>
-    <t>nadia.saadi@univ-alger.dz</t>
-  </si>
-  <si>
-    <t>Mourad</t>
-  </si>
-  <si>
-    <t>Khellaf</t>
-  </si>
-  <si>
-    <t>48291004</t>
-  </si>
-  <si>
-    <t>Mobile Development</t>
-  </si>
-  <si>
-    <t>0654321990</t>
-  </si>
-  <si>
-    <t>mourad.khellaf@univ-alger.dz</t>
-  </si>
-  <si>
-    <t>Saras</t>
-  </si>
-  <si>
-    <t>Djebber</t>
-  </si>
-  <si>
-    <t>48291003</t>
-  </si>
-  <si>
     <t>Artificial Intelligence</t>
   </si>
   <si>
-    <t>0654321989</t>
-  </si>
-  <si>
-    <t>sara.djebbar@univ-alger.dz</t>
-  </si>
-  <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
-    <t>Bouzid</t>
-  </si>
-  <si>
-    <t>48291002</t>
-  </si>
-  <si>
-    <t>Embedded Systems</t>
-  </si>
-  <si>
-    <t>0654321988</t>
-  </si>
-  <si>
-    <t>ahmed.bouzid@univ-alger.dz</t>
-  </si>
-  <si>
-    <t>Lina</t>
-  </si>
-  <si>
-    <t>Benali</t>
-  </si>
-  <si>
-    <t>48291001</t>
-  </si>
-  <si>
-    <t>Software Engineering</t>
-  </si>
-  <si>
-    <t>0654321987</t>
-  </si>
-  <si>
-    <t>lina.benali@univ-alger.dz</t>
-  </si>
-  <si>
-    <t>Sofia</t>
-  </si>
-  <si>
-    <t>Ait Kaci</t>
-  </si>
-  <si>
-    <t>31298745</t>
-  </si>
-  <si>
-    <t>0654987123</t>
-  </si>
-  <si>
-    <t>sofia.aitkaci@univ-boumerdes.dz</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/60</t>
-  </si>
-  <si>
     <t>Nour</t>
   </si>
   <si>
@@ -283,9 +142,6 @@
     <t>nour.hachemi@univ-tlemcen.dz</t>
   </si>
   <si>
-    <t>https://avatar.iran.liara.run/public/57</t>
-  </si>
-  <si>
     <t>Saheb</t>
   </si>
   <si>
@@ -301,9 +157,6 @@
     <t>amina.saheb@univ-guelma.dz</t>
   </si>
   <si>
-    <t>https://avatar.iran.liara.run/public/50</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -311,30 +164,6 @@
   </si>
   <si>
     <t>lastname</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/51</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/52</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/53</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/54</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/55</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/56</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/58</t>
-  </si>
-  <si>
-    <t>https://avatar.iran.liara.run/public/59</t>
   </si>
 </sst>
 </file>
@@ -345,13 +174,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -720,17 +549,26 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="9" width="31.6328125" customWidth="1"/>
+    <col min="10" max="10" width="63.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -757,10 +595,10 @@
         <v>7</v>
       </c>
       <c r="P1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -788,15 +626,16 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>93</v>
+      <c r="J2" t="str">
+        <f>_xlfn.CONCAT("https://api.dicebear.com/7.x/initials/svg?seed=",A2,B2)</f>
+        <v>https://api.dicebear.com/7.x/initials/svg?seed=YacineKerkar</v>
       </c>
       <c r="P2" t="str">
         <f>D2</f>
         <v>48291010</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -824,15 +663,16 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
-        <v>97</v>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J14" si="0">_xlfn.CONCAT("https://api.dicebear.com/7.x/initials/svg?seed=",A3,B3)</f>
+        <v>https://api.dicebear.com/7.x/initials/svg?seed=ImeneHaddad</v>
       </c>
       <c r="P3" t="str">
-        <f t="shared" ref="P3:P14" si="0">D3</f>
+        <f t="shared" ref="P3:P14" si="1">D3</f>
         <v>48291009</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -860,68 +700,70 @@
       <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" t="s">
-        <v>98</v>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://api.dicebear.com/7.x/initials/svg?seed=RachidBennour</v>
       </c>
       <c r="P4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48291008</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s">
-        <v>99</v>
-      </c>
-      <c r="P5" t="str">
-        <f t="shared" si="0"/>
-        <v>48291007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="J5" t="str">
+        <f>_xlfn.CONCAT("https://api.dicebear.com/7.x/initials/svg?seed=",A5,B5)</f>
+        <v>https://api.dicebear.com/7.x/initials/svg?seed=NourHachemi</v>
+      </c>
+      <c r="P5" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>42</v>
@@ -932,299 +774,60 @@
       <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" t="s">
-        <v>100</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="0"/>
-        <v>48291006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" t="s">
-        <v>101</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" si="0"/>
-        <v>48291005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" t="s">
-        <v>102</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="0"/>
-        <v>48291004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" t="s">
-        <v>87</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="0"/>
-        <v>48291003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" t="s">
-        <v>103</v>
-      </c>
-      <c r="P10" t="str">
-        <f t="shared" si="0"/>
-        <v>48291002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" t="s">
-        <v>104</v>
-      </c>
-      <c r="P11" t="str">
-        <f t="shared" si="0"/>
-        <v>48291001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" t="s">
-        <v>80</v>
-      </c>
-      <c r="P12" t="str">
-        <f t="shared" si="0"/>
-        <v>31298745</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" t="s">
-        <v>86</v>
-      </c>
-      <c r="J13" t="s">
-        <v>87</v>
-      </c>
+      <c r="J6" t="str">
+        <f>_xlfn.CONCAT("https://api.dicebear.com/7.x/initials/svg?seed=",A6,B6)</f>
+        <v>https://api.dicebear.com/7.x/initials/svg?seed=AminaSaheb</v>
+      </c>
+      <c r="P6" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P13" t="str">
-        <f t="shared" si="0"/>
+        <f>D5</f>
         <v>23987456</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I14" t="s">
-        <v>92</v>
-      </c>
-      <c r="J14" t="s">
-        <v>93</v>
-      </c>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P14" t="str">
-        <f t="shared" si="0"/>
+        <f>D6</f>
         <v>10495823</v>
       </c>
     </row>
@@ -1232,7 +835,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A12:J14 C1:J1 A2:I11" numberStoredAsText="1"/>
+    <ignoredError sqref="C1:J1 A2:I4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>